<commit_message>
Added number 2 in the 2nd cell
</commit_message>
<xml_diff>
--- a/table.xlsx
+++ b/table.xlsx
@@ -336,15 +336,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added number 3 in the 3rd cell
</commit_message>
<xml_diff>
--- a/table.xlsx
+++ b/table.xlsx
@@ -336,21 +336,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1">
         <v>2</v>
       </c>
+      <c r="C1">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added number 4 in the 4th cell
</commit_message>
<xml_diff>
--- a/table.xlsx
+++ b/table.xlsx
@@ -336,15 +336,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -354,6 +354,9 @@
       <c r="C1">
         <v>3</v>
       </c>
+      <c r="D1">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added number 5 in the 5th cell
</commit_message>
<xml_diff>
--- a/table.xlsx
+++ b/table.xlsx
@@ -336,10 +336,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -358,6 +358,11 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>